<commit_message>
i484--case export error wrong report dump
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/others/linux_LSE_engine_impl.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/others/linux_LSE_engine_impl.xlsx
@@ -5456,14 +5456,6 @@
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
 <headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{F777F3EB-26AC-4296-A7D5-AB64EF9CC2F9}" diskRevisions="1" revisionId="1496" version="23">
-  <header guid="{B28168CA-2211-49BD-883A-B5D210AAC0A8}" dateTime="2020-12-21T09:47:06" maxSheetId="5" userName="Jason Wang" r:id="rId22" minRId="1495">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
   <header guid="{F777F3EB-26AC-4296-A7D5-AB64EF9CC2F9}" dateTime="2020-12-21T09:47:49" maxSheetId="5" userName="Jason Wang" r:id="rId23" minRId="1496">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -5473,23 +5465,6 @@
     </sheetIdMap>
   </header>
 </headers>
-</file>
-
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="1495" sId="1">
-    <oc r="B7" t="inlineStr">
-      <is>
-        <t>cmd = python DEV/bin/run_radiant.py   --synthesis=lse   --run-map --sim-rtl --sim-syn-vlg --sim-questasim  --check-conf=sim.conf</t>
-      </is>
-    </oc>
-    <nc r="B7" t="inlineStr">
-      <is>
-        <t>cmd = python DEV/bin/run_radiant.py   --synthesis=lse   --run-map   --check-conf=impl.conf</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>